<commit_message>
Atualização relatório 4 - Mec Flu I
</commit_message>
<xml_diff>
--- a/Lab. Mec Flu I/Relatório_4/curva_calibração_CQ.xlsx
+++ b/Lab. Mec Flu I/Relatório_4/curva_calibração_CQ.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNESP\7-semestre-EngMec\Lab. Mec Flu I\Relatório_4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNESP\EngMec-UNESP\Lab. Mec Flu I\Relatório_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80ED6196-7B98-4DA0-A2C4-FD2646F8BCF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3DA54D1-7E86-484D-A823-0A205FAB4DDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{8754982A-341A-4262-BE93-CF9D7ED780C5}"/>
+    <workbookView xWindow="23424" yWindow="336" windowWidth="17280" windowHeight="9420" xr2:uid="{8754982A-341A-4262-BE93-CF9D7ED780C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -405,7 +405,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -441,6 +441,7 @@
       <c r="B4">
         <v>0.6855</v>
       </c>
+      <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
@@ -524,7 +525,7 @@
         <v>800000</v>
       </c>
       <c r="B14">
-        <v>0.67515000000000003</v>
+        <v>0.67512000000000005</v>
       </c>
       <c r="F14" s="3"/>
     </row>
@@ -533,7 +534,7 @@
         <v>900000</v>
       </c>
       <c r="B15">
-        <v>0.67515000000000003</v>
+        <v>0.67510000000000003</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -541,7 +542,7 @@
         <v>1000000</v>
       </c>
       <c r="B16">
-        <v>0.67515000000000003</v>
+        <v>0.67500000000000004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>